<commit_message>
plot fix, data fix
</commit_message>
<xml_diff>
--- a/Data/Параметры модели.xlsx
+++ b/Data/Параметры модели.xlsx
@@ -10865,28 +10865,28 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
         <x:v>36</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="I2" s="0" t="n">
-        <x:v>319</x:v>
+        <x:v>340</x:v>
       </x:c>
       <x:c r="J2" s="0" t="n">
         <x:v>0</x:v>
@@ -10903,28 +10903,28 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
         <x:v>275</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="I3" s="0" t="n">
-        <x:v>251</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="J3" s="0" t="n">
         <x:v>0</x:v>
@@ -10941,28 +10941,28 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
         <x:v>762</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>506</x:v>
+        <x:v>491</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="I4" s="0" t="n">
-        <x:v>421</x:v>
+        <x:v>394</x:v>
       </x:c>
       <x:c r="J4" s="0" t="n">
         <x:v>0</x:v>
@@ -10979,28 +10979,28 @@
         <x:v>81</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
         <x:v>600</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>399</x:v>
+        <x:v>376</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>25</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="I5" s="0" t="n">
-        <x:v>300</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="J5" s="0" t="n">
         <x:v>0</x:v>
@@ -11009,7 +11009,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="L5" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -11023,22 +11023,22 @@
         <x:v>1086</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>711</x:v>
+        <x:v>724</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>58</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="I6" s="0" t="n">
-        <x:v>435</x:v>
+        <x:v>461</x:v>
       </x:c>
       <x:c r="J6" s="0" t="n">
         <x:v>0</x:v>
@@ -11047,7 +11047,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="L6" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -11061,22 +11061,22 @@
         <x:v>986</x:v>
       </x:c>
       <x:c r="D7" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>645</x:v>
+        <x:v>655</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G7" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="I7" s="0" t="n">
-        <x:v>475</x:v>
+        <x:v>482</x:v>
       </x:c>
       <x:c r="J7" s="0" t="n">
         <x:v>0</x:v>
@@ -11099,22 +11099,22 @@
         <x:v>854</x:v>
       </x:c>
       <x:c r="D8" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>556</x:v>
+        <x:v>582</x:v>
       </x:c>
       <x:c r="F8" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G8" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="I8" s="0" t="n">
-        <x:v>220</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="J8" s="0" t="n">
         <x:v>0</x:v>
@@ -11123,7 +11123,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="L8" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -11137,22 +11137,22 @@
         <x:v>362</x:v>
       </x:c>
       <x:c r="D9" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E9" s="0" t="n">
-        <x:v>241</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F9" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G9" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="H9" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I9" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="J9" s="0" t="n">
         <x:v>0</x:v>
@@ -11161,7 +11161,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="L9" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -11175,22 +11175,22 @@
         <x:v>190</x:v>
       </x:c>
       <x:c r="D10" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="I10" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="J10" s="0" t="n">
         <x:v>0</x:v>
@@ -11199,7 +11199,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="L10" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>